<commit_message>
3.16.1 balance sheet tax
</commit_message>
<xml_diff>
--- a/docs/tc_demo_balance_sheet.xlsx
+++ b/docs/tc_demo_balance_sheet.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\company\trade control\apps\repos\tc-office\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB73815-E864-4449-88F8-3540F299E8F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C41FEF-707D-4951-8D86-EB4B57ADB34C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="1815" windowWidth="23880" windowHeight="12900" activeTab="1" xr2:uid="{F821936F-7F44-42E2-BCB5-A31DEFFCB6A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic" sheetId="9" r:id="rId1"/>
-    <sheet name="Advanced" sheetId="10" r:id="rId2"/>
+    <sheet name="Advanced" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="111">
   <si>
     <t>2019-20 (Closed)</t>
   </si>
@@ -342,42 +342,6 @@
     <t>CASH BOX</t>
   </si>
   <si>
-    <t>VAT QUARTERLY</t>
-  </si>
-  <si>
-    <t>Home Sales</t>
-  </si>
-  <si>
-    <t>Home Purchases</t>
-  </si>
-  <si>
-    <t>Export Sales</t>
-  </si>
-  <si>
-    <t>Export Purchases</t>
-  </si>
-  <si>
-    <t>Home Sales Vat</t>
-  </si>
-  <si>
-    <t>Home Purchases Vat</t>
-  </si>
-  <si>
-    <t>Export Sales Vat</t>
-  </si>
-  <si>
-    <t>Export Purchases Vat</t>
-  </si>
-  <si>
-    <t>Vat Adjustments</t>
-  </si>
-  <si>
-    <t>VAT DUE</t>
-  </si>
-  <si>
-    <t>VAT TOTALS</t>
-  </si>
-  <si>
     <t>PREMIS</t>
   </si>
   <si>
@@ -412,7 +376,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_);[Red]\(#,##0\)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,16 +454,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,12 +519,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDA70D6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -782,7 +732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -886,25 +836,6 @@
     </xf>
     <xf numFmtId="22" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="12" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12854,14 +12785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6906701-0868-461E-87F9-A2D21D834BE7}">
-  <dimension ref="A1:AQ144"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F06A0EB-50EC-4126-90A8-A0A81C62BB35}">
+  <dimension ref="A1:AQ121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="N119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="N92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -23022,7 +22953,7 @@
         <v>0</v>
       </c>
       <c r="AL93" s="23">
-        <v>-838.78</v>
+        <v>0</v>
       </c>
       <c r="AM93" s="23">
         <v>0</v>
@@ -23035,7 +22966,7 @@
       </c>
       <c r="AP93" s="5">
         <f>SUM(AD93:AO93)</f>
-        <v>-838.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:42" x14ac:dyDescent="0.2">
@@ -23214,7 +23145,7 @@
         <v>0</v>
       </c>
       <c r="Q95" s="23">
-        <v>0</v>
+        <v>522.45000000000005</v>
       </c>
       <c r="R95" s="23">
         <v>0</v>
@@ -23223,7 +23154,7 @@
         <v>0</v>
       </c>
       <c r="T95" s="23">
-        <v>0</v>
+        <v>1932.65</v>
       </c>
       <c r="U95" s="23">
         <v>0</v>
@@ -23232,7 +23163,7 @@
         <v>0</v>
       </c>
       <c r="W95" s="23">
-        <v>598</v>
+        <v>0</v>
       </c>
       <c r="X95" s="23">
         <v>0</v>
@@ -23241,7 +23172,7 @@
         <v>0</v>
       </c>
       <c r="Z95" s="23">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="AA95" s="23">
         <v>0</v>
@@ -23251,7 +23182,7 @@
       </c>
       <c r="AC95" s="5">
         <f>SUM(Q95:AB95)</f>
-        <v>903</v>
+        <v>2455.1000000000004</v>
       </c>
       <c r="AD95" s="23">
         <v>0</v>
@@ -23357,7 +23288,7 @@
       </c>
       <c r="Q96" s="34">
         <f>SUM(Q92:Q95)*-1</f>
-        <v>0</v>
+        <v>-522.45000000000005</v>
       </c>
       <c r="R96" s="34">
         <f>SUM(R92:R95)*-1</f>
@@ -23369,7 +23300,7 @@
       </c>
       <c r="T96" s="34">
         <f>SUM(T92:T95)*-1</f>
-        <v>0</v>
+        <v>-1932.65</v>
       </c>
       <c r="U96" s="34">
         <f>SUM(U92:U95)*-1</f>
@@ -23381,7 +23312,7 @@
       </c>
       <c r="W96" s="34">
         <f>SUM(W92:W95)*-1</f>
-        <v>-598</v>
+        <v>0</v>
       </c>
       <c r="X96" s="34">
         <f>SUM(X92:X95)*-1</f>
@@ -23393,7 +23324,7 @@
       </c>
       <c r="Z96" s="34">
         <f>SUM(Z92:Z95)*-1</f>
-        <v>-305</v>
+        <v>0</v>
       </c>
       <c r="AA96" s="34">
         <f>SUM(AA92:AA95)*-1</f>
@@ -23405,7 +23336,7 @@
       </c>
       <c r="AC96" s="35">
         <f>SUM(AC92:AC95)*-1</f>
-        <v>-903</v>
+        <v>-2455.1000000000004</v>
       </c>
       <c r="AD96" s="34">
         <f>SUM(AD92:AD95)*-1</f>
@@ -23441,7 +23372,7 @@
       </c>
       <c r="AL96" s="34">
         <f>SUM(AL92:AL95)*-1</f>
-        <v>838.78</v>
+        <v>0</v>
       </c>
       <c r="AM96" s="34">
         <f>SUM(AM92:AM95)*-1</f>
@@ -23457,7 +23388,7 @@
       </c>
       <c r="AP96" s="35">
         <f>SUM(AP92:AP95)*-1</f>
-        <v>838.78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:42" s="62" customFormat="1" x14ac:dyDescent="0.2">
@@ -23929,44 +23860,44 @@
         <v>6371.33</v>
       </c>
       <c r="Q103" s="23">
-        <v>5484.49</v>
+        <v>4962.0450000000001</v>
       </c>
       <c r="R103" s="23">
-        <v>2483.27</v>
+        <v>1960.825</v>
       </c>
       <c r="S103" s="23">
-        <v>8852.25</v>
+        <v>8329.8050000000003</v>
       </c>
       <c r="T103" s="23">
-        <v>7672.87</v>
+        <v>5217.7749999999996</v>
       </c>
       <c r="U103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="V103" s="24">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="W103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="X103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="Y103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="Z103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="AA103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="AB103" s="23">
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
       <c r="AC103" s="5">
         <f>AB103</f>
-        <v>7111.32</v>
+        <v>4656.2250000000004</v>
       </c>
     </row>
     <row r="104" spans="1:42" x14ac:dyDescent="0.2">
@@ -24198,55 +24129,55 @@
       </c>
       <c r="Q106" s="42">
         <f>SUM(Q103:Q105)</f>
-        <v>30817.73</v>
+        <v>30295.285</v>
       </c>
       <c r="R106" s="42">
         <f>SUM(R103:R105)</f>
-        <v>22637.200000000001</v>
+        <v>22114.755000000001</v>
       </c>
       <c r="S106" s="42">
         <f>SUM(S103:S105)</f>
-        <v>34004.629999999997</v>
+        <v>33482.184999999998</v>
       </c>
       <c r="T106" s="42">
         <f>SUM(T103:T105)</f>
-        <v>32673.25</v>
+        <v>30218.154999999999</v>
       </c>
       <c r="U106" s="42">
         <f>SUM(U103:U105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="V106" s="44">
         <f>SUM(V103:V105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="W106" s="42">
         <f>SUM(W103:W105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="X106" s="42">
         <f>SUM(X103:X105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="Y106" s="42">
         <f>SUM(Y103:Y105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="Z106" s="42">
         <f>SUM(Z103:Z105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="AA106" s="42">
         <f>SUM(AA103:AA105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="AB106" s="42">
         <f>SUM(AB103:AB105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="AC106" s="43">
         <f>SUM(AC103:AC105)</f>
-        <v>32975.94</v>
+        <v>30520.845000000001</v>
       </c>
       <c r="AD106" s="42">
         <f>SUM(AD103:AD105)</f>
@@ -24302,54 +24233,57 @@
       </c>
     </row>
     <row r="107" spans="1:42" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="108" spans="1:42" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="86" t="s">
-        <v>102</v>
-      </c>
-      <c r="B108" s="87"/>
-      <c r="C108" s="88"/>
-      <c r="D108" s="89"/>
-      <c r="E108" s="89"/>
-      <c r="F108" s="89"/>
-      <c r="G108" s="89"/>
-      <c r="H108" s="89"/>
-      <c r="I108" s="89"/>
-      <c r="J108" s="89"/>
-      <c r="K108" s="89"/>
-      <c r="L108" s="89"/>
-      <c r="M108" s="89"/>
-      <c r="N108" s="89"/>
-      <c r="O108" s="89"/>
-      <c r="P108" s="90"/>
-      <c r="Q108" s="89"/>
-      <c r="R108" s="89"/>
-      <c r="S108" s="89"/>
-      <c r="T108" s="89"/>
-      <c r="U108" s="89"/>
-      <c r="V108" s="89"/>
-      <c r="W108" s="89"/>
-      <c r="X108" s="89"/>
-      <c r="Y108" s="89"/>
-      <c r="Z108" s="89"/>
-      <c r="AA108" s="89"/>
-      <c r="AB108" s="89"/>
-      <c r="AC108" s="90"/>
-      <c r="AD108" s="89"/>
-      <c r="AE108" s="89"/>
-      <c r="AF108" s="89"/>
-      <c r="AG108" s="89"/>
-      <c r="AH108" s="89"/>
-      <c r="AI108" s="89"/>
-      <c r="AJ108" s="89"/>
-      <c r="AK108" s="89"/>
-      <c r="AL108" s="89"/>
-      <c r="AM108" s="89"/>
-      <c r="AN108" s="89"/>
-      <c r="AO108" s="89"/>
-      <c r="AP108" s="90"/>
+    <row r="108" spans="1:42" s="84" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="80" t="s">
+        <v>73</v>
+      </c>
+      <c r="B108" s="81"/>
+      <c r="C108" s="80"/>
+      <c r="D108" s="82"/>
+      <c r="E108" s="82"/>
+      <c r="F108" s="82"/>
+      <c r="G108" s="82"/>
+      <c r="H108" s="82"/>
+      <c r="I108" s="82"/>
+      <c r="J108" s="82"/>
+      <c r="K108" s="82"/>
+      <c r="L108" s="82"/>
+      <c r="M108" s="82"/>
+      <c r="N108" s="82"/>
+      <c r="O108" s="82"/>
+      <c r="P108" s="83"/>
+      <c r="Q108" s="82"/>
+      <c r="R108" s="82"/>
+      <c r="S108" s="82"/>
+      <c r="T108" s="82"/>
+      <c r="U108" s="82"/>
+      <c r="V108" s="82"/>
+      <c r="W108" s="82"/>
+      <c r="X108" s="82"/>
+      <c r="Y108" s="82"/>
+      <c r="Z108" s="82"/>
+      <c r="AA108" s="82"/>
+      <c r="AB108" s="82"/>
+      <c r="AC108" s="83"/>
+      <c r="AD108" s="82"/>
+      <c r="AE108" s="82"/>
+      <c r="AF108" s="82"/>
+      <c r="AG108" s="82"/>
+      <c r="AH108" s="82"/>
+      <c r="AI108" s="82"/>
+      <c r="AJ108" s="82"/>
+      <c r="AK108" s="82"/>
+      <c r="AL108" s="82"/>
+      <c r="AM108" s="82"/>
+      <c r="AN108" s="82"/>
+      <c r="AO108" s="82"/>
+      <c r="AP108" s="83"/>
     </row>
     <row r="109" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D109" s="23">
@@ -24383,100 +24317,63 @@
         <v>0</v>
       </c>
       <c r="N109" s="23">
-        <v>0</v>
+        <v>120000</v>
       </c>
       <c r="O109" s="23">
-        <v>5542.6949999999997</v>
+        <v>90000</v>
       </c>
       <c r="P109" s="5">
-        <f>SUM(D109:O109)</f>
-        <v>5542.6949999999997</v>
+        <f>O109</f>
+        <v>90000</v>
       </c>
       <c r="Q109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="R109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="S109" s="23">
-        <v>26010.33</v>
+        <v>90000</v>
       </c>
       <c r="T109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="U109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="V109" s="24">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="W109" s="23">
-        <v>4000</v>
+        <v>90000</v>
       </c>
       <c r="X109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Y109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="Z109" s="23">
-        <v>11365</v>
+        <v>90000</v>
       </c>
       <c r="AA109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="AB109" s="23">
-        <v>0</v>
+        <v>90000</v>
       </c>
       <c r="AC109" s="5">
-        <f>SUM(Q109:AB109)</f>
-        <v>41375.33</v>
-      </c>
-      <c r="AD109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO109" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP109" s="5">
-        <f>SUM(AD109:AO109)</f>
-        <v>0</v>
+        <f>AB109</f>
+        <v>90000</v>
       </c>
     </row>
     <row r="110" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>104</v>
       </c>
+      <c r="B110" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="D110" s="23">
         <v>0</v>
       </c>
@@ -24511,96 +24408,59 @@
         <v>0</v>
       </c>
       <c r="O110" s="23">
-        <v>6428.82</v>
+        <v>1000</v>
       </c>
       <c r="P110" s="5">
-        <f>SUM(D110:O110)</f>
-        <v>6428.82</v>
+        <f>O110</f>
+        <v>1000</v>
       </c>
       <c r="Q110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="R110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="S110" s="23">
-        <v>21765.01</v>
+        <v>1000</v>
       </c>
       <c r="T110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="U110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="V110" s="24">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="W110" s="23">
-        <v>2413.9</v>
+        <v>1000</v>
       </c>
       <c r="X110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Y110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="Z110" s="23">
-        <v>12765</v>
+        <v>1000</v>
       </c>
       <c r="AA110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AB110" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="AC110" s="5">
-        <f>SUM(Q110:AB110)</f>
-        <v>36943.910000000003</v>
-      </c>
-      <c r="AD110" s="23">
-        <v>3000</v>
-      </c>
-      <c r="AE110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO110" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP110" s="5">
-        <f>SUM(AD110:AO110)</f>
-        <v>3000</v>
+        <f>AB110</f>
+        <v>1000</v>
       </c>
     </row>
     <row r="111" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="D111" s="23">
         <v>0</v>
@@ -24636,96 +24496,59 @@
         <v>0</v>
       </c>
       <c r="O111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="P111" s="5">
-        <f>SUM(D111:O111)</f>
-        <v>0</v>
+        <f>O111</f>
+        <v>1250.25</v>
       </c>
       <c r="Q111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="R111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="S111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="T111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="U111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="V111" s="24">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="W111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="X111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="Y111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="Z111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="AA111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="AB111" s="23">
-        <v>0</v>
+        <v>1250.25</v>
       </c>
       <c r="AC111" s="5">
-        <f>SUM(Q111:AB111)</f>
-        <v>0</v>
-      </c>
-      <c r="AD111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO111" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP111" s="5">
-        <f>SUM(AD111:AO111)</f>
-        <v>0</v>
+        <f>AB111</f>
+        <v>1250.25</v>
       </c>
     </row>
     <row r="112" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="D112" s="23">
         <v>0</v>
@@ -24758,99 +24581,62 @@
         <v>0</v>
       </c>
       <c r="N112" s="23">
-        <v>0</v>
+        <v>1250</v>
       </c>
       <c r="O112" s="23">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="P112" s="5">
-        <f>SUM(D112:O112)</f>
-        <v>0</v>
+        <f>O112</f>
+        <v>1000</v>
       </c>
       <c r="Q112" s="23">
-        <v>0</v>
+        <v>1302</v>
       </c>
       <c r="R112" s="23">
-        <v>0</v>
+        <v>1177</v>
       </c>
       <c r="S112" s="23">
-        <v>0</v>
+        <v>2777</v>
       </c>
       <c r="T112" s="23">
-        <v>0</v>
+        <v>2144.2600000000002</v>
       </c>
       <c r="U112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="V112" s="24">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="W112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="X112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="Y112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="Z112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="AA112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="AB112" s="23">
-        <v>0</v>
+        <v>2279.52</v>
       </c>
       <c r="AC112" s="5">
-        <f>SUM(Q112:AB112)</f>
-        <v>0</v>
-      </c>
-      <c r="AD112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO112" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP112" s="5">
-        <f>SUM(AD112:AO112)</f>
-        <v>0</v>
+        <f>AB112</f>
+        <v>2279.52</v>
       </c>
     </row>
-    <row r="113" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>107</v>
+        <v>74</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="D113" s="23">
         <v>0</v>
@@ -24883,99 +24669,62 @@
         <v>0</v>
       </c>
       <c r="N113" s="23">
-        <v>0</v>
+        <v>25000</v>
       </c>
       <c r="O113" s="23">
-        <v>1108.5350000000001</v>
+        <v>24895</v>
       </c>
       <c r="P113" s="5">
-        <f>SUM(D113:O113)</f>
-        <v>1108.5350000000001</v>
+        <f>O113</f>
+        <v>24895</v>
       </c>
       <c r="Q113" s="23">
-        <v>0</v>
+        <v>24790</v>
       </c>
       <c r="R113" s="23">
-        <v>0</v>
+        <v>19685</v>
       </c>
       <c r="S113" s="23">
-        <v>5202.07</v>
+        <v>24580</v>
       </c>
       <c r="T113" s="23">
-        <v>0</v>
+        <v>24475</v>
       </c>
       <c r="U113" s="23">
-        <v>0</v>
+        <v>25370</v>
       </c>
       <c r="V113" s="24">
-        <v>0</v>
+        <v>25370</v>
       </c>
       <c r="W113" s="23">
-        <v>800</v>
+        <v>25370</v>
       </c>
       <c r="X113" s="23">
-        <v>0</v>
+        <v>25370</v>
       </c>
       <c r="Y113" s="23">
-        <v>0</v>
+        <v>25370</v>
       </c>
       <c r="Z113" s="23">
-        <v>2183</v>
+        <v>25370</v>
       </c>
       <c r="AA113" s="23">
-        <v>0</v>
+        <v>25370</v>
       </c>
       <c r="AB113" s="23">
-        <v>0</v>
+        <v>25370</v>
       </c>
       <c r="AC113" s="5">
-        <f>SUM(Q113:AB113)</f>
-        <v>8185.07</v>
-      </c>
-      <c r="AD113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO113" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP113" s="5">
-        <f>SUM(AD113:AO113)</f>
-        <v>0</v>
+        <f>AB113</f>
+        <v>25370</v>
       </c>
     </row>
-    <row r="114" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>108</v>
+        <v>76</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="D114" s="23">
         <v>0</v>
@@ -25008,2954 +24757,663 @@
         <v>0</v>
       </c>
       <c r="N114" s="23">
-        <v>0</v>
+        <v>8853.2999999999993</v>
       </c>
       <c r="O114" s="23">
-        <v>586.09</v>
+        <v>7066.31</v>
       </c>
       <c r="P114" s="5">
-        <f>SUM(D114:O114)</f>
-        <v>586.09</v>
+        <f>O114</f>
+        <v>7066.31</v>
       </c>
       <c r="Q114" s="23">
-        <v>0</v>
+        <v>5505.2849999999999</v>
       </c>
       <c r="R114" s="23">
-        <v>0</v>
+        <v>2429.7550000000001</v>
       </c>
       <c r="S114" s="23">
-        <v>3269.42</v>
+        <v>8902.1849999999995</v>
       </c>
       <c r="T114" s="23">
-        <v>0</v>
+        <v>5743.1549999999997</v>
       </c>
       <c r="U114" s="23">
-        <v>0</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="V114" s="24">
-        <v>0</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="W114" s="23">
-        <v>202</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="X114" s="23">
-        <v>0</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="Y114" s="23">
-        <v>0</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="Z114" s="23">
-        <v>1878</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="AA114" s="23">
-        <v>0</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="AB114" s="23">
-        <v>0</v>
+        <v>5150.8450000000003</v>
       </c>
       <c r="AC114" s="5">
-        <f>SUM(Q114:AB114)</f>
-        <v>5349.42</v>
-      </c>
-      <c r="AD114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO114" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP114" s="5">
-        <f>SUM(AD114:AO114)</f>
-        <v>0</v>
+        <f>AB114</f>
+        <v>5150.8450000000003</v>
       </c>
     </row>
-    <row r="115" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:43" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D115" s="23">
+        <v>0</v>
+      </c>
+      <c r="E115" s="23">
+        <v>0</v>
+      </c>
+      <c r="F115" s="23">
+        <v>0</v>
+      </c>
+      <c r="G115" s="23">
+        <v>0</v>
+      </c>
+      <c r="H115" s="23">
+        <v>0</v>
+      </c>
+      <c r="I115" s="23">
+        <v>0</v>
+      </c>
+      <c r="J115" s="23">
+        <v>0</v>
+      </c>
+      <c r="K115" s="23">
+        <v>0</v>
+      </c>
+      <c r="L115" s="23">
+        <v>0</v>
+      </c>
+      <c r="M115" s="23">
+        <v>0</v>
+      </c>
+      <c r="N115" s="23">
+        <v>2400</v>
+      </c>
+      <c r="O115" s="23">
+        <v>2400.0100000000002</v>
+      </c>
+      <c r="P115" s="5">
+        <f>O115</f>
+        <v>2400.0100000000002</v>
+      </c>
+      <c r="Q115" s="23">
+        <v>24600</v>
+      </c>
+      <c r="R115" s="23">
+        <v>24600</v>
+      </c>
+      <c r="S115" s="23">
+        <v>2400.0100000000002</v>
+      </c>
+      <c r="T115" s="23">
+        <v>3400.01</v>
+      </c>
+      <c r="U115" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="V115" s="24">
+        <v>0</v>
+      </c>
+      <c r="W115" s="23">
+        <v>0</v>
+      </c>
+      <c r="X115" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y115" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z115" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA115" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB115" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC115" s="5">
+        <f>AB115</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D115" s="23">
-        <v>0</v>
-      </c>
-      <c r="E115" s="23">
-        <v>0</v>
-      </c>
-      <c r="F115" s="23">
-        <v>0</v>
-      </c>
-      <c r="G115" s="23">
-        <v>0</v>
-      </c>
-      <c r="H115" s="23">
-        <v>0</v>
-      </c>
-      <c r="I115" s="23">
-        <v>0</v>
-      </c>
-      <c r="J115" s="23">
-        <v>0</v>
-      </c>
-      <c r="K115" s="23">
-        <v>0</v>
-      </c>
-      <c r="L115" s="23">
-        <v>0</v>
-      </c>
-      <c r="M115" s="23">
-        <v>0</v>
-      </c>
-      <c r="N115" s="23">
-        <v>0</v>
-      </c>
-      <c r="O115" s="23">
-        <v>0</v>
-      </c>
-      <c r="P115" s="5">
-        <f>SUM(D115:O115)</f>
-        <v>0</v>
-      </c>
-      <c r="Q115" s="23">
-        <v>0</v>
-      </c>
-      <c r="R115" s="23">
-        <v>0</v>
-      </c>
-      <c r="S115" s="23">
-        <v>0</v>
-      </c>
-      <c r="T115" s="23">
-        <v>0</v>
-      </c>
-      <c r="U115" s="23">
-        <v>0</v>
-      </c>
-      <c r="V115" s="24">
-        <v>0</v>
-      </c>
-      <c r="W115" s="23">
-        <v>0</v>
-      </c>
-      <c r="X115" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y115" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC115" s="5">
-        <f>SUM(Q115:AB115)</f>
-        <v>0</v>
-      </c>
-      <c r="AD115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO115" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP115" s="5">
-        <f>SUM(AD115:AO115)</f>
-        <v>0</v>
+      <c r="B116" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D116" s="23">
+        <v>0</v>
+      </c>
+      <c r="E116" s="23">
+        <v>0</v>
+      </c>
+      <c r="F116" s="23">
+        <v>0</v>
+      </c>
+      <c r="G116" s="23">
+        <v>0</v>
+      </c>
+      <c r="H116" s="23">
+        <v>0</v>
+      </c>
+      <c r="I116" s="23">
+        <v>0</v>
+      </c>
+      <c r="J116" s="23">
+        <v>0</v>
+      </c>
+      <c r="K116" s="23">
+        <v>0</v>
+      </c>
+      <c r="L116" s="23">
+        <v>0</v>
+      </c>
+      <c r="M116" s="23">
+        <v>0</v>
+      </c>
+      <c r="N116" s="23">
+        <v>-10000</v>
+      </c>
+      <c r="O116" s="23">
+        <v>-9900</v>
+      </c>
+      <c r="P116" s="5">
+        <f>O116</f>
+        <v>-9900</v>
+      </c>
+      <c r="Q116" s="23">
+        <v>-9800</v>
+      </c>
+      <c r="R116" s="23">
+        <v>-9700</v>
+      </c>
+      <c r="S116" s="23">
+        <v>-9600</v>
+      </c>
+      <c r="T116" s="23">
+        <v>-9500</v>
+      </c>
+      <c r="U116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="V116" s="24">
+        <v>-9400</v>
+      </c>
+      <c r="W116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="X116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="Y116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="Z116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="AA116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="AB116" s="23">
+        <v>-9400</v>
+      </c>
+      <c r="AC116" s="5">
+        <f>AB116</f>
+        <v>-9400</v>
       </c>
     </row>
-    <row r="116" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D116" s="23">
-        <v>0</v>
-      </c>
-      <c r="E116" s="23">
-        <v>0</v>
-      </c>
-      <c r="F116" s="23">
-        <v>0</v>
-      </c>
-      <c r="G116" s="23">
-        <v>0</v>
-      </c>
-      <c r="H116" s="23">
-        <v>0</v>
-      </c>
-      <c r="I116" s="23">
-        <v>0</v>
-      </c>
-      <c r="J116" s="23">
-        <v>0</v>
-      </c>
-      <c r="K116" s="23">
-        <v>0</v>
-      </c>
-      <c r="L116" s="23">
-        <v>0</v>
-      </c>
-      <c r="M116" s="23">
-        <v>0</v>
-      </c>
-      <c r="N116" s="23">
-        <v>0</v>
-      </c>
-      <c r="O116" s="23">
-        <v>0</v>
-      </c>
-      <c r="P116" s="5">
-        <f>SUM(D116:O116)</f>
-        <v>0</v>
-      </c>
-      <c r="Q116" s="23">
-        <v>0</v>
-      </c>
-      <c r="R116" s="23">
-        <v>0</v>
-      </c>
-      <c r="S116" s="23">
-        <v>0</v>
-      </c>
-      <c r="T116" s="23">
-        <v>0</v>
-      </c>
-      <c r="U116" s="23">
-        <v>0</v>
-      </c>
-      <c r="V116" s="24">
-        <v>0</v>
-      </c>
-      <c r="W116" s="23">
-        <v>0</v>
-      </c>
-      <c r="X116" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y116" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC116" s="5">
-        <f>SUM(Q116:AB116)</f>
-        <v>0</v>
-      </c>
-      <c r="AD116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO116" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP116" s="5">
-        <f>SUM(AD116:AO116)</f>
+    <row r="117" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D117" s="23">
+        <v>0</v>
+      </c>
+      <c r="E117" s="23">
+        <v>0</v>
+      </c>
+      <c r="F117" s="23">
+        <v>0</v>
+      </c>
+      <c r="G117" s="23">
+        <v>0</v>
+      </c>
+      <c r="H117" s="23">
+        <v>0</v>
+      </c>
+      <c r="I117" s="23">
+        <v>0</v>
+      </c>
+      <c r="J117" s="23">
+        <v>0</v>
+      </c>
+      <c r="K117" s="23">
+        <v>0</v>
+      </c>
+      <c r="L117" s="23">
+        <v>0</v>
+      </c>
+      <c r="M117" s="23">
+        <v>0</v>
+      </c>
+      <c r="N117" s="23">
+        <v>0</v>
+      </c>
+      <c r="O117" s="23">
+        <v>0</v>
+      </c>
+      <c r="P117" s="5">
+        <f>O117</f>
+        <v>0</v>
+      </c>
+      <c r="Q117" s="23">
+        <v>0</v>
+      </c>
+      <c r="R117" s="23">
+        <v>0</v>
+      </c>
+      <c r="S117" s="23">
+        <v>0</v>
+      </c>
+      <c r="T117" s="23">
+        <v>0</v>
+      </c>
+      <c r="U117" s="23">
+        <v>0</v>
+      </c>
+      <c r="V117" s="24">
+        <v>0</v>
+      </c>
+      <c r="W117" s="23">
+        <v>0</v>
+      </c>
+      <c r="X117" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y117" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z117" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA117" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB117" s="23">
+        <v>0</v>
+      </c>
+      <c r="AC117" s="5">
+        <f>AB117</f>
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A117" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D117" s="23">
-        <v>0</v>
-      </c>
-      <c r="E117" s="23">
-        <v>0</v>
-      </c>
-      <c r="F117" s="23">
-        <v>0</v>
-      </c>
-      <c r="G117" s="23">
-        <v>0</v>
-      </c>
-      <c r="H117" s="23">
-        <v>0</v>
-      </c>
-      <c r="I117" s="23">
-        <v>0</v>
-      </c>
-      <c r="J117" s="23">
-        <v>0</v>
-      </c>
-      <c r="K117" s="23">
-        <v>0</v>
-      </c>
-      <c r="L117" s="23">
-        <v>0</v>
-      </c>
-      <c r="M117" s="23">
-        <v>0</v>
-      </c>
-      <c r="N117" s="23">
-        <v>0</v>
-      </c>
-      <c r="O117" s="23">
-        <v>0</v>
-      </c>
-      <c r="P117" s="5">
-        <f>SUM(D117:O117)</f>
-        <v>0</v>
-      </c>
-      <c r="Q117" s="23">
-        <v>0</v>
-      </c>
-      <c r="R117" s="23">
-        <v>0</v>
-      </c>
-      <c r="S117" s="23">
-        <v>0</v>
-      </c>
-      <c r="T117" s="23">
-        <v>0</v>
-      </c>
-      <c r="U117" s="23">
-        <v>0</v>
-      </c>
-      <c r="V117" s="24">
-        <v>0</v>
-      </c>
-      <c r="W117" s="23">
-        <v>0</v>
-      </c>
-      <c r="X117" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y117" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC117" s="5">
-        <f>SUM(Q117:AB117)</f>
-        <v>0</v>
-      </c>
-      <c r="AD117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO117" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP117" s="5">
-        <f>SUM(AD117:AO117)</f>
-        <v>0</v>
+    <row r="118" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D118" s="23">
+        <v>0</v>
+      </c>
+      <c r="E118" s="23">
+        <v>0</v>
+      </c>
+      <c r="F118" s="23">
+        <v>0</v>
+      </c>
+      <c r="G118" s="23">
+        <v>0</v>
+      </c>
+      <c r="H118" s="23">
+        <v>0</v>
+      </c>
+      <c r="I118" s="23">
+        <v>0</v>
+      </c>
+      <c r="J118" s="23">
+        <v>0</v>
+      </c>
+      <c r="K118" s="23">
+        <v>0</v>
+      </c>
+      <c r="L118" s="23">
+        <v>0</v>
+      </c>
+      <c r="M118" s="23">
+        <v>0</v>
+      </c>
+      <c r="N118" s="23">
+        <v>0</v>
+      </c>
+      <c r="O118" s="23">
+        <v>0</v>
+      </c>
+      <c r="P118" s="5">
+        <f>O118</f>
+        <v>0</v>
+      </c>
+      <c r="Q118" s="23">
+        <v>0</v>
+      </c>
+      <c r="R118" s="23">
+        <v>0</v>
+      </c>
+      <c r="S118" s="23">
+        <v>0</v>
+      </c>
+      <c r="T118" s="23">
+        <v>0</v>
+      </c>
+      <c r="U118" s="23">
+        <v>0</v>
+      </c>
+      <c r="V118" s="24">
+        <v>0</v>
+      </c>
+      <c r="W118" s="23">
+        <v>0</v>
+      </c>
+      <c r="X118" s="23">
+        <v>-445.68</v>
+      </c>
+      <c r="Y118" s="23">
+        <v>-445.68</v>
+      </c>
+      <c r="Z118" s="23">
+        <v>-445.68</v>
+      </c>
+      <c r="AA118" s="23">
+        <v>-445.68</v>
+      </c>
+      <c r="AB118" s="23">
+        <v>-445.68</v>
+      </c>
+      <c r="AC118" s="5">
+        <f>AB118</f>
+        <v>-445.68</v>
       </c>
     </row>
-    <row r="118" spans="1:42" s="94" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="B118" s="41"/>
-      <c r="C118" s="40"/>
-      <c r="D118" s="92">
-        <v>0</v>
-      </c>
-      <c r="E118" s="92">
-        <v>0</v>
-      </c>
-      <c r="F118" s="92">
-        <v>0</v>
-      </c>
-      <c r="G118" s="92">
-        <v>0</v>
-      </c>
-      <c r="H118" s="92">
-        <v>0</v>
-      </c>
-      <c r="I118" s="92">
-        <v>0</v>
-      </c>
-      <c r="J118" s="92">
-        <v>0</v>
-      </c>
-      <c r="K118" s="92">
-        <v>0</v>
-      </c>
-      <c r="L118" s="92">
-        <v>0</v>
-      </c>
-      <c r="M118" s="92">
-        <v>0</v>
-      </c>
-      <c r="N118" s="92">
-        <v>0</v>
-      </c>
-      <c r="O118" s="92">
-        <v>522.44500000000005</v>
-      </c>
-      <c r="P118" s="43">
-        <f>SUM(D118:O118)</f>
-        <v>522.44500000000005</v>
-      </c>
-      <c r="Q118" s="92">
-        <v>0</v>
-      </c>
-      <c r="R118" s="92">
-        <v>0</v>
-      </c>
-      <c r="S118" s="92">
-        <v>1932.65</v>
-      </c>
-      <c r="T118" s="92">
-        <v>0</v>
-      </c>
-      <c r="U118" s="92">
-        <v>0</v>
-      </c>
-      <c r="V118" s="93">
-        <v>0</v>
-      </c>
-      <c r="W118" s="92">
-        <v>598</v>
-      </c>
-      <c r="X118" s="92">
-        <v>0</v>
-      </c>
-      <c r="Y118" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z118" s="92">
-        <v>305</v>
-      </c>
-      <c r="AA118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AC118" s="43">
-        <f>SUM(Q118:AB118)</f>
-        <v>2835.65</v>
-      </c>
-      <c r="AD118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AE118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AF118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AG118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AH118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AI118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AJ118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AK118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AL118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AM118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AN118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AO118" s="92">
-        <v>0</v>
-      </c>
-      <c r="AP118" s="43">
-        <f>SUM(AD118:AO118)</f>
-        <v>0</v>
+    <row r="119" spans="1:43" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D119" s="23">
+        <v>0</v>
+      </c>
+      <c r="E119" s="23">
+        <v>0</v>
+      </c>
+      <c r="F119" s="23">
+        <v>0</v>
+      </c>
+      <c r="G119" s="23">
+        <v>0</v>
+      </c>
+      <c r="H119" s="23">
+        <v>0</v>
+      </c>
+      <c r="I119" s="23">
+        <v>0</v>
+      </c>
+      <c r="J119" s="23">
+        <v>0</v>
+      </c>
+      <c r="K119" s="23">
+        <v>0</v>
+      </c>
+      <c r="L119" s="23">
+        <v>0</v>
+      </c>
+      <c r="M119" s="23">
+        <v>0</v>
+      </c>
+      <c r="N119" s="23">
+        <v>-830</v>
+      </c>
+      <c r="O119" s="23">
+        <v>-1830</v>
+      </c>
+      <c r="P119" s="5">
+        <f>O119</f>
+        <v>-1830</v>
+      </c>
+      <c r="Q119" s="23">
+        <v>-19729.994999999999</v>
+      </c>
+      <c r="R119" s="23">
+        <v>-11879.994999999999</v>
+      </c>
+      <c r="S119" s="23">
+        <v>-1045.355</v>
+      </c>
+      <c r="T119" s="23">
+        <v>-1313.5550000000001</v>
+      </c>
+      <c r="U119" s="23">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="V119" s="24">
+        <v>-1000.005</v>
+      </c>
+      <c r="W119" s="23">
+        <v>-1000</v>
+      </c>
+      <c r="X119" s="23">
+        <v>-1000</v>
+      </c>
+      <c r="Y119" s="23">
+        <v>-1000</v>
+      </c>
+      <c r="Z119" s="23">
+        <v>-1000</v>
+      </c>
+      <c r="AA119" s="23">
+        <v>-1000</v>
+      </c>
+      <c r="AB119" s="23">
+        <v>-1000</v>
+      </c>
+      <c r="AC119" s="5">
+        <f>AB119</f>
+        <v>-1000</v>
       </c>
     </row>
-    <row r="119" spans="1:42" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="1:42" s="91" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="86" t="s">
-        <v>113</v>
-      </c>
-      <c r="B120" s="87"/>
-      <c r="C120" s="88"/>
-      <c r="D120" s="89"/>
-      <c r="E120" s="89"/>
-      <c r="F120" s="89"/>
-      <c r="G120" s="89"/>
-      <c r="H120" s="89"/>
-      <c r="I120" s="89"/>
-      <c r="J120" s="89"/>
-      <c r="K120" s="89"/>
-      <c r="L120" s="89"/>
-      <c r="M120" s="89"/>
-      <c r="N120" s="89"/>
-      <c r="O120" s="89"/>
-      <c r="P120" s="90"/>
-      <c r="Q120" s="89"/>
-      <c r="R120" s="89"/>
-      <c r="S120" s="89"/>
-      <c r="T120" s="89"/>
-      <c r="U120" s="89"/>
-      <c r="V120" s="89"/>
-      <c r="W120" s="89"/>
-      <c r="X120" s="89"/>
-      <c r="Y120" s="89"/>
-      <c r="Z120" s="89"/>
-      <c r="AA120" s="89"/>
-      <c r="AB120" s="89"/>
-      <c r="AC120" s="90"/>
-      <c r="AD120" s="89"/>
-      <c r="AE120" s="89"/>
-      <c r="AF120" s="89"/>
-      <c r="AG120" s="89"/>
-      <c r="AH120" s="89"/>
-      <c r="AI120" s="89"/>
-      <c r="AJ120" s="89"/>
-      <c r="AK120" s="89"/>
-      <c r="AL120" s="89"/>
-      <c r="AM120" s="89"/>
-      <c r="AN120" s="89"/>
-      <c r="AO120" s="89"/>
-      <c r="AP120" s="90"/>
+    <row r="120" spans="1:43" s="40" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="B120" s="41"/>
+      <c r="D120" s="42">
+        <f>SUM(D109:D119)</f>
+        <v>0</v>
+      </c>
+      <c r="E120" s="42">
+        <f>SUM(E109:E119)</f>
+        <v>0</v>
+      </c>
+      <c r="F120" s="42">
+        <f>SUM(F109:F119)</f>
+        <v>0</v>
+      </c>
+      <c r="G120" s="42">
+        <f>SUM(G109:G119)</f>
+        <v>0</v>
+      </c>
+      <c r="H120" s="42">
+        <f>SUM(H109:H119)</f>
+        <v>0</v>
+      </c>
+      <c r="I120" s="42">
+        <f>SUM(I109:I119)</f>
+        <v>0</v>
+      </c>
+      <c r="J120" s="42">
+        <f>SUM(J109:J119)</f>
+        <v>0</v>
+      </c>
+      <c r="K120" s="42">
+        <f>SUM(K109:K119)</f>
+        <v>0</v>
+      </c>
+      <c r="L120" s="42">
+        <f>SUM(L109:L119)</f>
+        <v>0</v>
+      </c>
+      <c r="M120" s="42">
+        <f>SUM(M109:M119)</f>
+        <v>0</v>
+      </c>
+      <c r="N120" s="42">
+        <f>SUM(N109:N119)</f>
+        <v>146673.29999999999</v>
+      </c>
+      <c r="O120" s="42">
+        <f>SUM(O109:O119)</f>
+        <v>115881.56999999999</v>
+      </c>
+      <c r="P120" s="43">
+        <f>O120</f>
+        <v>115881.56999999999</v>
+      </c>
+      <c r="Q120" s="42">
+        <f>SUM(Q109:Q119)</f>
+        <v>118917.54000000001</v>
+      </c>
+      <c r="R120" s="42">
+        <f>SUM(R109:R119)</f>
+        <v>118562.01000000001</v>
+      </c>
+      <c r="S120" s="42">
+        <f>SUM(S109:S119)</f>
+        <v>120264.09</v>
+      </c>
+      <c r="T120" s="42">
+        <f>SUM(T109:T119)</f>
+        <v>117199.12</v>
+      </c>
+      <c r="U120" s="42">
+        <f>SUM(U109:U119)</f>
+        <v>115650.62</v>
+      </c>
+      <c r="V120" s="44">
+        <f>SUM(V109:V119)</f>
+        <v>114650.61</v>
+      </c>
+      <c r="W120" s="42">
+        <f>SUM(W109:W119)</f>
+        <v>114650.61500000001</v>
+      </c>
+      <c r="X120" s="42">
+        <f>SUM(X109:X119)</f>
+        <v>114204.93500000001</v>
+      </c>
+      <c r="Y120" s="42">
+        <f>SUM(Y109:Y119)</f>
+        <v>114204.93500000001</v>
+      </c>
+      <c r="Z120" s="42">
+        <f>SUM(Z109:Z119)</f>
+        <v>114204.93500000001</v>
+      </c>
+      <c r="AA120" s="42">
+        <f>SUM(AA109:AA119)</f>
+        <v>114204.93500000001</v>
+      </c>
+      <c r="AB120" s="42">
+        <f>SUM(AB109:AB119)</f>
+        <v>114204.93500000001</v>
+      </c>
+      <c r="AC120" s="43">
+        <f>AB120</f>
+        <v>114204.93500000001</v>
+      </c>
+      <c r="AD120" s="42">
+        <f>SUM(AD109:AD119)</f>
+        <v>0</v>
+      </c>
+      <c r="AE120" s="42">
+        <f>SUM(AE109:AE119)</f>
+        <v>0</v>
+      </c>
+      <c r="AF120" s="42">
+        <f>SUM(AF109:AF119)</f>
+        <v>0</v>
+      </c>
+      <c r="AG120" s="42">
+        <f>SUM(AG109:AG119)</f>
+        <v>0</v>
+      </c>
+      <c r="AH120" s="42">
+        <f>SUM(AH109:AH119)</f>
+        <v>0</v>
+      </c>
+      <c r="AI120" s="42">
+        <f>SUM(AI109:AI119)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ120" s="42">
+        <f>SUM(AJ109:AJ119)</f>
+        <v>0</v>
+      </c>
+      <c r="AK120" s="42">
+        <f>SUM(AK109:AK119)</f>
+        <v>0</v>
+      </c>
+      <c r="AL120" s="42">
+        <f>SUM(AL109:AL119)</f>
+        <v>0</v>
+      </c>
+      <c r="AM120" s="42">
+        <f>SUM(AM109:AM119)</f>
+        <v>0</v>
+      </c>
+      <c r="AN120" s="42">
+        <f>SUM(AN109:AN119)</f>
+        <v>0</v>
+      </c>
+      <c r="AO120" s="42">
+        <f>SUM(AO109:AO119)</f>
+        <v>0</v>
+      </c>
+      <c r="AP120" s="43">
+        <f>AO120</f>
+        <v>0</v>
+      </c>
+      <c r="AQ120" s="40">
+        <f>SUM(AQ109:AQ119)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="121" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A121" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D121" s="23">
-        <v>0</v>
-      </c>
-      <c r="E121" s="23">
-        <v>0</v>
-      </c>
-      <c r="F121" s="23">
-        <v>0</v>
-      </c>
-      <c r="G121" s="23">
-        <v>0</v>
-      </c>
-      <c r="H121" s="23">
-        <v>0</v>
-      </c>
-      <c r="I121" s="23">
-        <v>0</v>
-      </c>
-      <c r="J121" s="23">
-        <v>0</v>
-      </c>
-      <c r="K121" s="23">
-        <v>0</v>
-      </c>
-      <c r="L121" s="23">
-        <v>0</v>
-      </c>
-      <c r="M121" s="23">
-        <v>0</v>
-      </c>
-      <c r="N121" s="23">
-        <v>2821.67</v>
-      </c>
-      <c r="O121" s="23">
-        <v>2721.0250000000001</v>
-      </c>
-      <c r="P121" s="5">
-        <f>SUM(D121:O121)</f>
-        <v>5542.6949999999997</v>
-      </c>
-      <c r="Q121" s="23">
-        <v>20969.38</v>
-      </c>
-      <c r="R121" s="23">
-        <v>2354.7399999999998</v>
-      </c>
-      <c r="S121" s="23">
-        <v>2686.21</v>
-      </c>
-      <c r="T121" s="23">
-        <v>2210.83</v>
-      </c>
-      <c r="U121" s="23">
-        <v>2307.6999999999998</v>
-      </c>
-      <c r="V121" s="24">
-        <v>2000</v>
-      </c>
-      <c r="W121" s="23">
-        <v>1865</v>
-      </c>
-      <c r="X121" s="23">
-        <v>9500</v>
-      </c>
-      <c r="Y121" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC121" s="5">
-        <f>SUM(Q121:AB121)</f>
-        <v>43893.86</v>
-      </c>
-      <c r="AD121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO121" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP121" s="5">
-        <f>SUM(AD121:AO121)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A122" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D122" s="23">
-        <v>0</v>
-      </c>
-      <c r="E122" s="23">
-        <v>0</v>
-      </c>
-      <c r="F122" s="23">
-        <v>0</v>
-      </c>
-      <c r="G122" s="23">
-        <v>0</v>
-      </c>
-      <c r="H122" s="23">
-        <v>0</v>
-      </c>
-      <c r="I122" s="23">
-        <v>0</v>
-      </c>
-      <c r="J122" s="23">
-        <v>0</v>
-      </c>
-      <c r="K122" s="23">
-        <v>0</v>
-      </c>
-      <c r="L122" s="23">
-        <v>0</v>
-      </c>
-      <c r="M122" s="23">
-        <v>0</v>
-      </c>
-      <c r="N122" s="23">
-        <v>1923.9</v>
-      </c>
-      <c r="O122" s="23">
-        <v>4504.92</v>
-      </c>
-      <c r="P122" s="5">
-        <f>SUM(D122:O122)</f>
-        <v>6428.82</v>
-      </c>
-      <c r="Q122" s="23">
-        <v>17698.22</v>
-      </c>
-      <c r="R122" s="23">
-        <v>2012.52</v>
-      </c>
-      <c r="S122" s="23">
-        <v>2054.27</v>
-      </c>
-      <c r="T122" s="23">
-        <v>2097.5500000000002</v>
-      </c>
-      <c r="U122" s="23">
-        <v>1840</v>
-      </c>
-      <c r="V122" s="24">
-        <v>1613.9</v>
-      </c>
-      <c r="W122" s="23">
-        <v>2375</v>
-      </c>
-      <c r="X122" s="23">
-        <v>9390</v>
-      </c>
-      <c r="Y122" s="23">
-        <v>1000</v>
-      </c>
-      <c r="Z122" s="23">
-        <v>1000</v>
-      </c>
-      <c r="AA122" s="23">
-        <v>1000</v>
-      </c>
-      <c r="AB122" s="23">
-        <v>1000</v>
-      </c>
-      <c r="AC122" s="5">
-        <f>SUM(Q122:AB122)</f>
-        <v>43081.460000000006</v>
-      </c>
-      <c r="AD122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO122" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP122" s="5">
-        <f>SUM(AD122:AO122)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A123" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D123" s="23">
-        <v>0</v>
-      </c>
-      <c r="E123" s="23">
-        <v>0</v>
-      </c>
-      <c r="F123" s="23">
-        <v>0</v>
-      </c>
-      <c r="G123" s="23">
-        <v>0</v>
-      </c>
-      <c r="H123" s="23">
-        <v>0</v>
-      </c>
-      <c r="I123" s="23">
-        <v>0</v>
-      </c>
-      <c r="J123" s="23">
-        <v>0</v>
-      </c>
-      <c r="K123" s="23">
-        <v>0</v>
-      </c>
-      <c r="L123" s="23">
-        <v>0</v>
-      </c>
-      <c r="M123" s="23">
-        <v>0</v>
-      </c>
-      <c r="N123" s="23">
-        <v>0</v>
-      </c>
-      <c r="O123" s="23">
-        <v>0</v>
-      </c>
-      <c r="P123" s="5">
-        <f>SUM(D123:O123)</f>
-        <v>0</v>
-      </c>
-      <c r="Q123" s="23">
-        <v>0</v>
-      </c>
-      <c r="R123" s="23">
-        <v>0</v>
-      </c>
-      <c r="S123" s="23">
-        <v>0</v>
-      </c>
-      <c r="T123" s="23">
-        <v>0</v>
-      </c>
-      <c r="U123" s="23">
-        <v>0</v>
-      </c>
-      <c r="V123" s="24">
-        <v>0</v>
-      </c>
-      <c r="W123" s="23">
-        <v>0</v>
-      </c>
-      <c r="X123" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y123" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC123" s="5">
-        <f>SUM(Q123:AB123)</f>
-        <v>0</v>
-      </c>
-      <c r="AD123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO123" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP123" s="5">
-        <f>SUM(AD123:AO123)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A124" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D124" s="23">
-        <v>0</v>
-      </c>
-      <c r="E124" s="23">
-        <v>0</v>
-      </c>
-      <c r="F124" s="23">
-        <v>0</v>
-      </c>
-      <c r="G124" s="23">
-        <v>0</v>
-      </c>
-      <c r="H124" s="23">
-        <v>0</v>
-      </c>
-      <c r="I124" s="23">
-        <v>0</v>
-      </c>
-      <c r="J124" s="23">
-        <v>0</v>
-      </c>
-      <c r="K124" s="23">
-        <v>0</v>
-      </c>
-      <c r="L124" s="23">
-        <v>0</v>
-      </c>
-      <c r="M124" s="23">
-        <v>0</v>
-      </c>
-      <c r="N124" s="23">
-        <v>0</v>
-      </c>
-      <c r="O124" s="23">
-        <v>0</v>
-      </c>
-      <c r="P124" s="5">
-        <f>SUM(D124:O124)</f>
-        <v>0</v>
-      </c>
-      <c r="Q124" s="23">
-        <v>0</v>
-      </c>
-      <c r="R124" s="23">
-        <v>0</v>
-      </c>
-      <c r="S124" s="23">
-        <v>0</v>
-      </c>
-      <c r="T124" s="23">
-        <v>0</v>
-      </c>
-      <c r="U124" s="23">
-        <v>0</v>
-      </c>
-      <c r="V124" s="24">
-        <v>0</v>
-      </c>
-      <c r="W124" s="23">
-        <v>0</v>
-      </c>
-      <c r="X124" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y124" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC124" s="5">
-        <f>SUM(Q124:AB124)</f>
-        <v>0</v>
-      </c>
-      <c r="AD124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO124" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP124" s="5">
-        <f>SUM(AD124:AO124)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A125" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D125" s="23">
-        <v>0</v>
-      </c>
-      <c r="E125" s="23">
-        <v>0</v>
-      </c>
-      <c r="F125" s="23">
-        <v>0</v>
-      </c>
-      <c r="G125" s="23">
-        <v>0</v>
-      </c>
-      <c r="H125" s="23">
-        <v>0</v>
-      </c>
-      <c r="I125" s="23">
-        <v>0</v>
-      </c>
-      <c r="J125" s="23">
-        <v>0</v>
-      </c>
-      <c r="K125" s="23">
-        <v>0</v>
-      </c>
-      <c r="L125" s="23">
-        <v>0</v>
-      </c>
-      <c r="M125" s="23">
-        <v>0</v>
-      </c>
-      <c r="N125" s="23">
-        <v>564.33000000000004</v>
-      </c>
-      <c r="O125" s="23">
-        <v>544.20500000000004</v>
-      </c>
-      <c r="P125" s="5">
-        <f>SUM(D125:O125)</f>
-        <v>1108.5350000000001</v>
-      </c>
-      <c r="Q125" s="23">
-        <v>4193.88</v>
-      </c>
-      <c r="R125" s="23">
-        <v>470.95</v>
-      </c>
-      <c r="S125" s="23">
-        <v>537.24</v>
-      </c>
-      <c r="T125" s="23">
-        <v>442.17</v>
-      </c>
-      <c r="U125" s="23">
-        <v>461.54</v>
-      </c>
-      <c r="V125" s="24">
-        <v>400</v>
-      </c>
-      <c r="W125" s="23">
-        <v>283</v>
-      </c>
-      <c r="X125" s="23">
-        <v>1900</v>
-      </c>
-      <c r="Y125" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC125" s="5">
-        <f>SUM(Q125:AB125)</f>
-        <v>8688.7799999999988</v>
-      </c>
-      <c r="AD125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO125" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP125" s="5">
-        <f>SUM(AD125:AO125)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A126" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D126" s="23">
-        <v>0</v>
-      </c>
-      <c r="E126" s="23">
-        <v>0</v>
-      </c>
-      <c r="F126" s="23">
-        <v>0</v>
-      </c>
-      <c r="G126" s="23">
-        <v>0</v>
-      </c>
-      <c r="H126" s="23">
-        <v>0</v>
-      </c>
-      <c r="I126" s="23">
-        <v>0</v>
-      </c>
-      <c r="J126" s="23">
-        <v>0</v>
-      </c>
-      <c r="K126" s="23">
-        <v>0</v>
-      </c>
-      <c r="L126" s="23">
-        <v>0</v>
-      </c>
-      <c r="M126" s="23">
-        <v>0</v>
-      </c>
-      <c r="N126" s="23">
-        <v>38.799999999999997</v>
-      </c>
-      <c r="O126" s="23">
-        <v>547.29</v>
-      </c>
-      <c r="P126" s="5">
-        <f>SUM(D126:O126)</f>
-        <v>586.08999999999992</v>
-      </c>
-      <c r="Q126" s="23">
-        <v>3188.62</v>
-      </c>
-      <c r="R126" s="23">
-        <v>38.700000000000003</v>
-      </c>
-      <c r="S126" s="23">
-        <v>42.1</v>
-      </c>
-      <c r="T126" s="23">
-        <v>50.03</v>
-      </c>
-      <c r="U126" s="23">
-        <v>38</v>
-      </c>
-      <c r="V126" s="24">
-        <v>172</v>
-      </c>
-      <c r="W126" s="23">
-        <v>200</v>
-      </c>
-      <c r="X126" s="23">
-        <v>1678</v>
-      </c>
-      <c r="Y126" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC126" s="5">
-        <f>SUM(Q126:AB126)</f>
-        <v>5407.45</v>
-      </c>
-      <c r="AD126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO126" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP126" s="5">
-        <f>SUM(AD126:AO126)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A127" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D127" s="23">
-        <v>0</v>
-      </c>
-      <c r="E127" s="23">
-        <v>0</v>
-      </c>
-      <c r="F127" s="23">
-        <v>0</v>
-      </c>
-      <c r="G127" s="23">
-        <v>0</v>
-      </c>
-      <c r="H127" s="23">
-        <v>0</v>
-      </c>
-      <c r="I127" s="23">
-        <v>0</v>
-      </c>
-      <c r="J127" s="23">
-        <v>0</v>
-      </c>
-      <c r="K127" s="23">
-        <v>0</v>
-      </c>
-      <c r="L127" s="23">
-        <v>0</v>
-      </c>
-      <c r="M127" s="23">
-        <v>0</v>
-      </c>
-      <c r="N127" s="23">
-        <v>0</v>
-      </c>
-      <c r="O127" s="23">
-        <v>0</v>
-      </c>
-      <c r="P127" s="5">
-        <f>SUM(D127:O127)</f>
-        <v>0</v>
-      </c>
-      <c r="Q127" s="23">
-        <v>0</v>
-      </c>
-      <c r="R127" s="23">
-        <v>0</v>
-      </c>
-      <c r="S127" s="23">
-        <v>0</v>
-      </c>
-      <c r="T127" s="23">
-        <v>0</v>
-      </c>
-      <c r="U127" s="23">
-        <v>0</v>
-      </c>
-      <c r="V127" s="24">
-        <v>0</v>
-      </c>
-      <c r="W127" s="23">
-        <v>0</v>
-      </c>
-      <c r="X127" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y127" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC127" s="5">
-        <f>SUM(Q127:AB127)</f>
-        <v>0</v>
-      </c>
-      <c r="AD127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO127" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP127" s="5">
-        <f>SUM(AD127:AO127)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A128" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D128" s="23">
-        <v>0</v>
-      </c>
-      <c r="E128" s="23">
-        <v>0</v>
-      </c>
-      <c r="F128" s="23">
-        <v>0</v>
-      </c>
-      <c r="G128" s="23">
-        <v>0</v>
-      </c>
-      <c r="H128" s="23">
-        <v>0</v>
-      </c>
-      <c r="I128" s="23">
-        <v>0</v>
-      </c>
-      <c r="J128" s="23">
-        <v>0</v>
-      </c>
-      <c r="K128" s="23">
-        <v>0</v>
-      </c>
-      <c r="L128" s="23">
-        <v>0</v>
-      </c>
-      <c r="M128" s="23">
-        <v>0</v>
-      </c>
-      <c r="N128" s="23">
-        <v>0</v>
-      </c>
-      <c r="O128" s="23">
-        <v>0</v>
-      </c>
-      <c r="P128" s="5">
-        <f>SUM(D128:O128)</f>
-        <v>0</v>
-      </c>
-      <c r="Q128" s="23">
-        <v>0</v>
-      </c>
-      <c r="R128" s="23">
-        <v>0</v>
-      </c>
-      <c r="S128" s="23">
-        <v>0</v>
-      </c>
-      <c r="T128" s="23">
-        <v>0</v>
-      </c>
-      <c r="U128" s="23">
-        <v>0</v>
-      </c>
-      <c r="V128" s="24">
-        <v>0</v>
-      </c>
-      <c r="W128" s="23">
-        <v>0</v>
-      </c>
-      <c r="X128" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y128" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC128" s="5">
-        <f>SUM(Q128:AB128)</f>
-        <v>0</v>
-      </c>
-      <c r="AD128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AE128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AF128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AG128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AH128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AI128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AJ128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AK128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AL128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AM128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AN128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AO128" s="23">
-        <v>0</v>
-      </c>
-      <c r="AP128" s="5">
-        <f>SUM(AD128:AO128)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:43" s="94" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="B129" s="41"/>
-      <c r="C129" s="40"/>
-      <c r="D129" s="92">
-        <v>0</v>
-      </c>
-      <c r="E129" s="92">
-        <v>0</v>
-      </c>
-      <c r="F129" s="92">
-        <v>0</v>
-      </c>
-      <c r="G129" s="92">
-        <v>0</v>
-      </c>
-      <c r="H129" s="92">
-        <v>0</v>
-      </c>
-      <c r="I129" s="92">
-        <v>0</v>
-      </c>
-      <c r="J129" s="92">
-        <v>0</v>
-      </c>
-      <c r="K129" s="92">
-        <v>0</v>
-      </c>
-      <c r="L129" s="92">
-        <v>0</v>
-      </c>
-      <c r="M129" s="92">
-        <v>0</v>
-      </c>
-      <c r="N129" s="92">
-        <v>525.53</v>
-      </c>
-      <c r="O129" s="92">
-        <v>-3.085</v>
-      </c>
-      <c r="P129" s="43">
-        <f>SUM(D129:O129)</f>
-        <v>522.44499999999994</v>
-      </c>
-      <c r="Q129" s="92">
-        <v>1005.26</v>
-      </c>
-      <c r="R129" s="92">
-        <v>432.25</v>
-      </c>
-      <c r="S129" s="92">
-        <v>495.14</v>
-      </c>
-      <c r="T129" s="92">
-        <v>392.14</v>
-      </c>
-      <c r="U129" s="92">
-        <v>423.54</v>
-      </c>
-      <c r="V129" s="93">
-        <v>228</v>
-      </c>
-      <c r="W129" s="92">
-        <v>83</v>
-      </c>
-      <c r="X129" s="92">
-        <v>222</v>
-      </c>
-      <c r="Y129" s="92">
-        <v>0</v>
-      </c>
-      <c r="Z129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AA129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AB129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AC129" s="43">
-        <f>SUM(Q129:AB129)</f>
-        <v>3281.33</v>
-      </c>
-      <c r="AD129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AE129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AF129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AG129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AH129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AI129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AJ129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AK129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AL129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AM129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AN129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AO129" s="92">
-        <v>0</v>
-      </c>
-      <c r="AP129" s="43">
-        <f>SUM(AD129:AO129)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:43" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="131" spans="1:43" s="84" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A131" s="80" t="s">
-        <v>73</v>
-      </c>
-      <c r="B131" s="81"/>
-      <c r="C131" s="80"/>
-      <c r="D131" s="82"/>
-      <c r="E131" s="82"/>
-      <c r="F131" s="82"/>
-      <c r="G131" s="82"/>
-      <c r="H131" s="82"/>
-      <c r="I131" s="82"/>
-      <c r="J131" s="82"/>
-      <c r="K131" s="82"/>
-      <c r="L131" s="82"/>
-      <c r="M131" s="82"/>
-      <c r="N131" s="82"/>
-      <c r="O131" s="82"/>
-      <c r="P131" s="83"/>
-      <c r="Q131" s="82"/>
-      <c r="R131" s="82"/>
-      <c r="S131" s="82"/>
-      <c r="T131" s="82"/>
-      <c r="U131" s="82"/>
-      <c r="V131" s="82"/>
-      <c r="W131" s="82"/>
-      <c r="X131" s="82"/>
-      <c r="Y131" s="82"/>
-      <c r="Z131" s="82"/>
-      <c r="AA131" s="82"/>
-      <c r="AB131" s="82"/>
-      <c r="AC131" s="83"/>
-      <c r="AD131" s="82"/>
-      <c r="AE131" s="82"/>
-      <c r="AF131" s="82"/>
-      <c r="AG131" s="82"/>
-      <c r="AH131" s="82"/>
-      <c r="AI131" s="82"/>
-      <c r="AJ131" s="82"/>
-      <c r="AK131" s="82"/>
-      <c r="AL131" s="82"/>
-      <c r="AM131" s="82"/>
-      <c r="AN131" s="82"/>
-      <c r="AO131" s="82"/>
-      <c r="AP131" s="83"/>
-    </row>
-    <row r="132" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A132" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B132" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D132" s="23">
-        <v>0</v>
-      </c>
-      <c r="E132" s="23">
-        <v>0</v>
-      </c>
-      <c r="F132" s="23">
-        <v>0</v>
-      </c>
-      <c r="G132" s="23">
-        <v>0</v>
-      </c>
-      <c r="H132" s="23">
-        <v>0</v>
-      </c>
-      <c r="I132" s="23">
-        <v>0</v>
-      </c>
-      <c r="J132" s="23">
-        <v>0</v>
-      </c>
-      <c r="K132" s="23">
-        <v>0</v>
-      </c>
-      <c r="L132" s="23">
-        <v>0</v>
-      </c>
-      <c r="M132" s="23">
-        <v>0</v>
-      </c>
-      <c r="N132" s="23">
-        <v>120000</v>
-      </c>
-      <c r="O132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="P132" s="5">
-        <f>O132</f>
-        <v>90000</v>
-      </c>
-      <c r="Q132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="R132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="S132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="T132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="U132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="V132" s="24">
-        <v>90000</v>
-      </c>
-      <c r="W132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="X132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="Y132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="Z132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="AA132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="AB132" s="23">
-        <v>90000</v>
-      </c>
-      <c r="AC132" s="5">
-        <f>AB132</f>
-        <v>90000</v>
-      </c>
-    </row>
-    <row r="133" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A133" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B133" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D133" s="23">
-        <v>0</v>
-      </c>
-      <c r="E133" s="23">
-        <v>0</v>
-      </c>
-      <c r="F133" s="23">
-        <v>0</v>
-      </c>
-      <c r="G133" s="23">
-        <v>0</v>
-      </c>
-      <c r="H133" s="23">
-        <v>0</v>
-      </c>
-      <c r="I133" s="23">
-        <v>0</v>
-      </c>
-      <c r="J133" s="23">
-        <v>0</v>
-      </c>
-      <c r="K133" s="23">
-        <v>0</v>
-      </c>
-      <c r="L133" s="23">
-        <v>0</v>
-      </c>
-      <c r="M133" s="23">
-        <v>0</v>
-      </c>
-      <c r="N133" s="23">
-        <v>0</v>
-      </c>
-      <c r="O133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="P133" s="5">
-        <f>O133</f>
-        <v>1000</v>
-      </c>
-      <c r="Q133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="R133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="S133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="T133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="U133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="V133" s="24">
-        <v>1000</v>
-      </c>
-      <c r="W133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="X133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="Y133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="Z133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="AA133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="AB133" s="23">
-        <v>1000</v>
-      </c>
-      <c r="AC133" s="5">
-        <f>AB133</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="134" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A134" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B134" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D134" s="23">
-        <v>0</v>
-      </c>
-      <c r="E134" s="23">
-        <v>0</v>
-      </c>
-      <c r="F134" s="23">
-        <v>0</v>
-      </c>
-      <c r="G134" s="23">
-        <v>0</v>
-      </c>
-      <c r="H134" s="23">
-        <v>0</v>
-      </c>
-      <c r="I134" s="23">
-        <v>0</v>
-      </c>
-      <c r="J134" s="23">
-        <v>0</v>
-      </c>
-      <c r="K134" s="23">
-        <v>0</v>
-      </c>
-      <c r="L134" s="23">
-        <v>0</v>
-      </c>
-      <c r="M134" s="23">
-        <v>0</v>
-      </c>
-      <c r="N134" s="23">
-        <v>0</v>
-      </c>
-      <c r="O134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="P134" s="5">
-        <f>O134</f>
-        <v>1250.25</v>
-      </c>
-      <c r="Q134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="R134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="S134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="T134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="U134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="V134" s="24">
-        <v>1250.25</v>
-      </c>
-      <c r="W134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="X134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="Y134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="Z134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="AA134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="AB134" s="23">
-        <v>1250.25</v>
-      </c>
-      <c r="AC134" s="5">
-        <f>AB134</f>
-        <v>1250.25</v>
-      </c>
-    </row>
-    <row r="135" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="D135" s="23">
-        <v>0</v>
-      </c>
-      <c r="E135" s="23">
-        <v>0</v>
-      </c>
-      <c r="F135" s="23">
-        <v>0</v>
-      </c>
-      <c r="G135" s="23">
-        <v>0</v>
-      </c>
-      <c r="H135" s="23">
-        <v>0</v>
-      </c>
-      <c r="I135" s="23">
-        <v>0</v>
-      </c>
-      <c r="J135" s="23">
-        <v>0</v>
-      </c>
-      <c r="K135" s="23">
-        <v>0</v>
-      </c>
-      <c r="L135" s="23">
-        <v>0</v>
-      </c>
-      <c r="M135" s="23">
-        <v>0</v>
-      </c>
-      <c r="N135" s="23">
-        <v>1250</v>
-      </c>
-      <c r="O135" s="23">
-        <v>1000</v>
-      </c>
-      <c r="P135" s="5">
-        <f>O135</f>
-        <v>1000</v>
-      </c>
-      <c r="Q135" s="23">
-        <v>1302</v>
-      </c>
-      <c r="R135" s="23">
-        <v>1177</v>
-      </c>
-      <c r="S135" s="23">
-        <v>2777</v>
-      </c>
-      <c r="T135" s="23">
-        <v>2144.2600000000002</v>
-      </c>
-      <c r="U135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="V135" s="24">
-        <v>2279.52</v>
-      </c>
-      <c r="W135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="X135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="Y135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="Z135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="AA135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="AB135" s="23">
-        <v>2279.52</v>
-      </c>
-      <c r="AC135" s="5">
-        <f>AB135</f>
-        <v>2279.52</v>
-      </c>
-    </row>
-    <row r="136" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A136" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D136" s="23">
-        <v>0</v>
-      </c>
-      <c r="E136" s="23">
-        <v>0</v>
-      </c>
-      <c r="F136" s="23">
-        <v>0</v>
-      </c>
-      <c r="G136" s="23">
-        <v>0</v>
-      </c>
-      <c r="H136" s="23">
-        <v>0</v>
-      </c>
-      <c r="I136" s="23">
-        <v>0</v>
-      </c>
-      <c r="J136" s="23">
-        <v>0</v>
-      </c>
-      <c r="K136" s="23">
-        <v>0</v>
-      </c>
-      <c r="L136" s="23">
-        <v>0</v>
-      </c>
-      <c r="M136" s="23">
-        <v>0</v>
-      </c>
-      <c r="N136" s="23">
-        <v>25000</v>
-      </c>
-      <c r="O136" s="23">
-        <v>24895</v>
-      </c>
-      <c r="P136" s="5">
-        <f>O136</f>
-        <v>24895</v>
-      </c>
-      <c r="Q136" s="23">
-        <v>24790</v>
-      </c>
-      <c r="R136" s="23">
-        <v>19685</v>
-      </c>
-      <c r="S136" s="23">
-        <v>24580</v>
-      </c>
-      <c r="T136" s="23">
-        <v>24475</v>
-      </c>
-      <c r="U136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="V136" s="24">
-        <v>25370</v>
-      </c>
-      <c r="W136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="X136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="Y136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="Z136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="AA136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="AB136" s="23">
-        <v>25370</v>
-      </c>
-      <c r="AC136" s="5">
-        <f>AB136</f>
-        <v>25370</v>
-      </c>
-    </row>
-    <row r="137" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D137" s="23">
-        <v>0</v>
-      </c>
-      <c r="E137" s="23">
-        <v>0</v>
-      </c>
-      <c r="F137" s="23">
-        <v>0</v>
-      </c>
-      <c r="G137" s="23">
-        <v>0</v>
-      </c>
-      <c r="H137" s="23">
-        <v>0</v>
-      </c>
-      <c r="I137" s="23">
-        <v>0</v>
-      </c>
-      <c r="J137" s="23">
-        <v>0</v>
-      </c>
-      <c r="K137" s="23">
-        <v>0</v>
-      </c>
-      <c r="L137" s="23">
-        <v>0</v>
-      </c>
-      <c r="M137" s="23">
-        <v>0</v>
-      </c>
-      <c r="N137" s="23">
-        <v>8853.2999999999993</v>
-      </c>
-      <c r="O137" s="23">
-        <v>7066.31</v>
-      </c>
-      <c r="P137" s="5">
-        <f>O137</f>
-        <v>7066.31</v>
-      </c>
-      <c r="Q137" s="23">
-        <v>6027.73</v>
-      </c>
-      <c r="R137" s="23">
-        <v>2952.2</v>
-      </c>
-      <c r="S137" s="23">
-        <v>9424.6299999999992</v>
-      </c>
-      <c r="T137" s="23">
-        <v>8198.25</v>
-      </c>
-      <c r="U137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="V137" s="24">
-        <v>7605.94</v>
-      </c>
-      <c r="W137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="X137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="Y137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="Z137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="AA137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="AB137" s="23">
-        <v>7605.94</v>
-      </c>
-      <c r="AC137" s="5">
-        <f>AB137</f>
-        <v>7605.94</v>
-      </c>
-    </row>
-    <row r="138" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D138" s="23">
-        <v>0</v>
-      </c>
-      <c r="E138" s="23">
-        <v>0</v>
-      </c>
-      <c r="F138" s="23">
-        <v>0</v>
-      </c>
-      <c r="G138" s="23">
-        <v>0</v>
-      </c>
-      <c r="H138" s="23">
-        <v>0</v>
-      </c>
-      <c r="I138" s="23">
-        <v>0</v>
-      </c>
-      <c r="J138" s="23">
-        <v>0</v>
-      </c>
-      <c r="K138" s="23">
-        <v>0</v>
-      </c>
-      <c r="L138" s="23">
-        <v>0</v>
-      </c>
-      <c r="M138" s="23">
-        <v>0</v>
-      </c>
-      <c r="N138" s="23">
-        <v>2400</v>
-      </c>
-      <c r="O138" s="23">
-        <v>2400.0100000000002</v>
-      </c>
-      <c r="P138" s="5">
-        <f>O138</f>
-        <v>2400.0100000000002</v>
-      </c>
-      <c r="Q138" s="23">
-        <v>24600</v>
-      </c>
-      <c r="R138" s="23">
-        <v>24600</v>
-      </c>
-      <c r="S138" s="23">
-        <v>2400.0100000000002</v>
-      </c>
-      <c r="T138" s="23">
-        <v>3400.01</v>
-      </c>
-      <c r="U138" s="23">
-        <v>0.01</v>
-      </c>
-      <c r="V138" s="24">
-        <v>0</v>
-      </c>
-      <c r="W138" s="23">
-        <v>0</v>
-      </c>
-      <c r="X138" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y138" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z138" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA138" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB138" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC138" s="5">
-        <f>AB138</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A139" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D139" s="23">
-        <v>0</v>
-      </c>
-      <c r="E139" s="23">
-        <v>0</v>
-      </c>
-      <c r="F139" s="23">
-        <v>0</v>
-      </c>
-      <c r="G139" s="23">
-        <v>0</v>
-      </c>
-      <c r="H139" s="23">
-        <v>0</v>
-      </c>
-      <c r="I139" s="23">
-        <v>0</v>
-      </c>
-      <c r="J139" s="23">
-        <v>0</v>
-      </c>
-      <c r="K139" s="23">
-        <v>0</v>
-      </c>
-      <c r="L139" s="23">
-        <v>0</v>
-      </c>
-      <c r="M139" s="23">
-        <v>0</v>
-      </c>
-      <c r="N139" s="23">
-        <v>-10000</v>
-      </c>
-      <c r="O139" s="23">
-        <v>-9900</v>
-      </c>
-      <c r="P139" s="5">
-        <f>O139</f>
-        <v>-9900</v>
-      </c>
-      <c r="Q139" s="23">
-        <v>-9800</v>
-      </c>
-      <c r="R139" s="23">
-        <v>-9700</v>
-      </c>
-      <c r="S139" s="23">
-        <v>-9600</v>
-      </c>
-      <c r="T139" s="23">
-        <v>-9500</v>
-      </c>
-      <c r="U139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="V139" s="24">
-        <v>-9400</v>
-      </c>
-      <c r="W139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="X139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="Y139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="Z139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="AA139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="AB139" s="23">
-        <v>-9400</v>
-      </c>
-      <c r="AC139" s="5">
-        <f>AB139</f>
-        <v>-9400</v>
-      </c>
-    </row>
-    <row r="140" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A140" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D140" s="23">
-        <v>0</v>
-      </c>
-      <c r="E140" s="23">
-        <v>0</v>
-      </c>
-      <c r="F140" s="23">
-        <v>0</v>
-      </c>
-      <c r="G140" s="23">
-        <v>0</v>
-      </c>
-      <c r="H140" s="23">
-        <v>0</v>
-      </c>
-      <c r="I140" s="23">
-        <v>0</v>
-      </c>
-      <c r="J140" s="23">
-        <v>0</v>
-      </c>
-      <c r="K140" s="23">
-        <v>0</v>
-      </c>
-      <c r="L140" s="23">
-        <v>0</v>
-      </c>
-      <c r="M140" s="23">
-        <v>0</v>
-      </c>
-      <c r="N140" s="23">
-        <v>0</v>
-      </c>
-      <c r="O140" s="23">
-        <v>0</v>
-      </c>
-      <c r="P140" s="5">
-        <f>O140</f>
-        <v>0</v>
-      </c>
-      <c r="Q140" s="23">
-        <v>0</v>
-      </c>
-      <c r="R140" s="23">
-        <v>0</v>
-      </c>
-      <c r="S140" s="23">
-        <v>0</v>
-      </c>
-      <c r="T140" s="23">
-        <v>0</v>
-      </c>
-      <c r="U140" s="23">
-        <v>0</v>
-      </c>
-      <c r="V140" s="24">
-        <v>0</v>
-      </c>
-      <c r="W140" s="23">
-        <v>0</v>
-      </c>
-      <c r="X140" s="23">
-        <v>0</v>
-      </c>
-      <c r="Y140" s="23">
-        <v>0</v>
-      </c>
-      <c r="Z140" s="23">
-        <v>577.22499000000005</v>
-      </c>
-      <c r="AA140" s="23">
-        <v>577.22499000000005</v>
-      </c>
-      <c r="AB140" s="23">
-        <v>577.22499000000005</v>
-      </c>
-      <c r="AC140" s="5">
-        <f>AB140</f>
-        <v>577.22499000000005</v>
-      </c>
-    </row>
-    <row r="141" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A141" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D141" s="23">
-        <v>0</v>
-      </c>
-      <c r="E141" s="23">
-        <v>0</v>
-      </c>
-      <c r="F141" s="23">
-        <v>0</v>
-      </c>
-      <c r="G141" s="23">
-        <v>0</v>
-      </c>
-      <c r="H141" s="23">
-        <v>0</v>
-      </c>
-      <c r="I141" s="23">
-        <v>0</v>
-      </c>
-      <c r="J141" s="23">
-        <v>0</v>
-      </c>
-      <c r="K141" s="23">
-        <v>0</v>
-      </c>
-      <c r="L141" s="23">
-        <v>0</v>
-      </c>
-      <c r="M141" s="23">
-        <v>0</v>
-      </c>
-      <c r="N141" s="23">
-        <v>0</v>
-      </c>
-      <c r="O141" s="23">
-        <v>0</v>
-      </c>
-      <c r="P141" s="5">
-        <f>O141</f>
-        <v>0</v>
-      </c>
-      <c r="Q141" s="23">
-        <v>0</v>
-      </c>
-      <c r="R141" s="23">
-        <v>-522.44499999999994</v>
-      </c>
-      <c r="S141" s="23">
-        <v>-522.44499999999994</v>
-      </c>
-      <c r="T141" s="23">
-        <v>-522.44499999999994</v>
-      </c>
-      <c r="U141" s="23">
-        <v>-2455.0950000000003</v>
-      </c>
-      <c r="V141" s="24">
-        <v>-2455.0950000000003</v>
-      </c>
-      <c r="W141" s="23">
-        <v>-2455.0950000000003</v>
-      </c>
-      <c r="X141" s="23">
-        <v>-2900.7750000000001</v>
-      </c>
-      <c r="Y141" s="23">
-        <v>-2900.7750000000001</v>
-      </c>
-      <c r="Z141" s="23">
-        <v>-2900.7750000000001</v>
-      </c>
-      <c r="AA141" s="23">
-        <v>-2900.7750000000001</v>
-      </c>
-      <c r="AB141" s="23">
-        <v>-2900.7750000000001</v>
-      </c>
-      <c r="AC141" s="5">
-        <f>AB141</f>
-        <v>-2900.7750000000001</v>
-      </c>
-    </row>
-    <row r="142" spans="1:43" x14ac:dyDescent="0.2">
-      <c r="A142" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D142" s="23">
-        <v>0</v>
-      </c>
-      <c r="E142" s="23">
-        <v>0</v>
-      </c>
-      <c r="F142" s="23">
-        <v>0</v>
-      </c>
-      <c r="G142" s="23">
-        <v>0</v>
-      </c>
-      <c r="H142" s="23">
-        <v>0</v>
-      </c>
-      <c r="I142" s="23">
-        <v>0</v>
-      </c>
-      <c r="J142" s="23">
-        <v>0</v>
-      </c>
-      <c r="K142" s="23">
-        <v>0</v>
-      </c>
-      <c r="L142" s="23">
-        <v>0</v>
-      </c>
-      <c r="M142" s="23">
-        <v>0</v>
-      </c>
-      <c r="N142" s="23">
-        <v>-830</v>
-      </c>
-      <c r="O142" s="23">
-        <v>-1830</v>
-      </c>
-      <c r="P142" s="5">
-        <f>O142</f>
-        <v>-1830</v>
-      </c>
-      <c r="Q142" s="23">
-        <v>-19729.989999999998</v>
-      </c>
-      <c r="R142" s="23">
-        <v>-11879.99</v>
-      </c>
-      <c r="S142" s="23">
-        <v>-1045.3499999999999</v>
-      </c>
-      <c r="T142" s="23">
-        <v>-1313.55</v>
-      </c>
-      <c r="U142" s="23">
-        <v>-1313.55</v>
-      </c>
-      <c r="V142" s="24">
-        <v>-1000</v>
-      </c>
-      <c r="W142" s="23">
-        <v>-1000</v>
-      </c>
-      <c r="X142" s="23">
-        <v>-1000</v>
-      </c>
-      <c r="Y142" s="23">
-        <v>-1000</v>
-      </c>
-      <c r="Z142" s="23">
-        <v>-1000</v>
-      </c>
-      <c r="AA142" s="23">
-        <v>-1000</v>
-      </c>
-      <c r="AB142" s="23">
-        <v>-1000</v>
-      </c>
-      <c r="AC142" s="5">
-        <f>AB142</f>
-        <v>-1000</v>
-      </c>
-    </row>
-    <row r="143" spans="1:43" s="40" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="B143" s="41"/>
-      <c r="D143" s="42">
-        <f>SUM(D132:D142)</f>
-        <v>0</v>
-      </c>
-      <c r="E143" s="42">
-        <f>SUM(E132:E142)</f>
-        <v>0</v>
-      </c>
-      <c r="F143" s="42">
-        <f>SUM(F132:F142)</f>
-        <v>0</v>
-      </c>
-      <c r="G143" s="42">
-        <f>SUM(G132:G142)</f>
-        <v>0</v>
-      </c>
-      <c r="H143" s="42">
-        <f>SUM(H132:H142)</f>
-        <v>0</v>
-      </c>
-      <c r="I143" s="42">
-        <f>SUM(I132:I142)</f>
-        <v>0</v>
-      </c>
-      <c r="J143" s="42">
-        <f>SUM(J132:J142)</f>
-        <v>0</v>
-      </c>
-      <c r="K143" s="42">
-        <f>SUM(K132:K142)</f>
-        <v>0</v>
-      </c>
-      <c r="L143" s="42">
-        <f>SUM(L132:L142)</f>
-        <v>0</v>
-      </c>
-      <c r="M143" s="42">
-        <f>SUM(M132:M142)</f>
-        <v>0</v>
-      </c>
-      <c r="N143" s="42">
-        <f>SUM(N132:N142)</f>
-        <v>146673.29999999999</v>
-      </c>
-      <c r="O143" s="42">
-        <f>SUM(O132:O142)</f>
-        <v>115881.56999999999</v>
-      </c>
-      <c r="P143" s="43">
-        <f>O143</f>
-        <v>115881.56999999999</v>
-      </c>
-      <c r="Q143" s="42">
-        <f>SUM(Q132:Q142)</f>
-        <v>119439.98999999999</v>
-      </c>
-      <c r="R143" s="42">
-        <f>SUM(R132:R142)</f>
-        <v>118562.015</v>
-      </c>
-      <c r="S143" s="42">
-        <f>SUM(S132:S142)</f>
-        <v>120264.095</v>
-      </c>
-      <c r="T143" s="42">
-        <f>SUM(T132:T142)</f>
-        <v>119131.77499999998</v>
-      </c>
-      <c r="U143" s="42">
-        <f>SUM(U132:U142)</f>
-        <v>114337.075</v>
-      </c>
-      <c r="V143" s="44">
-        <f>SUM(V132:V142)</f>
-        <v>114650.61500000001</v>
-      </c>
-      <c r="W143" s="42">
-        <f>SUM(W132:W142)</f>
-        <v>114650.61500000001</v>
-      </c>
-      <c r="X143" s="42">
-        <f>SUM(X132:X142)</f>
-        <v>114204.93500000001</v>
-      </c>
-      <c r="Y143" s="42">
-        <f>SUM(Y132:Y142)</f>
-        <v>114204.93500000001</v>
-      </c>
-      <c r="Z143" s="42">
-        <f>SUM(Z132:Z142)</f>
-        <v>114782.15999000001</v>
-      </c>
-      <c r="AA143" s="42">
-        <f>SUM(AA132:AA142)</f>
-        <v>114782.15999000001</v>
-      </c>
-      <c r="AB143" s="42">
-        <f>SUM(AB132:AB142)</f>
-        <v>114782.15999000001</v>
-      </c>
-      <c r="AC143" s="43">
-        <f>AB143</f>
-        <v>114782.15999000001</v>
-      </c>
-      <c r="AD143" s="42">
-        <f>SUM(AD132:AD142)</f>
-        <v>0</v>
-      </c>
-      <c r="AE143" s="42">
-        <f>SUM(AE132:AE142)</f>
-        <v>0</v>
-      </c>
-      <c r="AF143" s="42">
-        <f>SUM(AF132:AF142)</f>
-        <v>0</v>
-      </c>
-      <c r="AG143" s="42">
-        <f>SUM(AG132:AG142)</f>
-        <v>0</v>
-      </c>
-      <c r="AH143" s="42">
-        <f>SUM(AH132:AH142)</f>
-        <v>0</v>
-      </c>
-      <c r="AI143" s="42">
-        <f>SUM(AI132:AI142)</f>
-        <v>0</v>
-      </c>
-      <c r="AJ143" s="42">
-        <f>SUM(AJ132:AJ142)</f>
-        <v>0</v>
-      </c>
-      <c r="AK143" s="42">
-        <f>SUM(AK132:AK142)</f>
-        <v>0</v>
-      </c>
-      <c r="AL143" s="42">
-        <f>SUM(AL132:AL142)</f>
-        <v>0</v>
-      </c>
-      <c r="AM143" s="42">
-        <f>SUM(AM132:AM142)</f>
-        <v>0</v>
-      </c>
-      <c r="AN143" s="42">
-        <f>SUM(AN132:AN142)</f>
-        <v>0</v>
-      </c>
-      <c r="AO143" s="42">
-        <f>SUM(AO132:AO142)</f>
-        <v>0</v>
-      </c>
-      <c r="AP143" s="43">
-        <f>AO143</f>
-        <v>0</v>
-      </c>
-      <c r="AQ143" s="40">
-        <f>SUM(AQ132:AQ142)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:43" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="121" spans="1:43" ht="12" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <dataConsolidate/>

</xml_diff>